<commit_message>
Added "GoTo" dialogue functionality
Dialogue can now be seamlessly transitioned from one conversation to another.
-Added "SECTION_ID" which can be used for (hopefully) different sub-menus with important NPCs.
-Added "GOTO_CONVERSATION", "GOTO_SECTION", and "GOTO_LINE" to be able to make certain lines chain back or forward.
-Added "Exit", which specifies whether or not you want this line of dialogue to quit the dialogue early. Good for certain GOTOs that you want to transition.

This is all me throwing stuff together, so code/conceptual review is needed for this.
</commit_message>
<xml_diff>
--- a/PostIMDgame/Content/NPC/DataStructure/DialogueXCL.xlsx
+++ b/PostIMDgame/Content/NPC/DataStructure/DialogueXCL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Users\aleks\Documents\GitHub\Post-IMD\PostIMDgame\Content\NPC\DataStructure\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8A99A65C-037D-4B69-B57C-5DAC0E6DCE3E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B5A9869-CA9C-45E6-A128-667A6A537D61}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3930" yWindow="2985" windowWidth="21600" windowHeight="11385" xr2:uid="{18883775-5A3F-46B9-9AFF-2C5EA3946A2B}"/>
+    <workbookView xWindow="-25320" yWindow="270" windowWidth="25440" windowHeight="15390" xr2:uid="{18883775-5A3F-46B9-9AFF-2C5EA3946A2B}"/>
   </bookViews>
   <sheets>
     <sheet name="DialogueCSV" sheetId="1" r:id="rId1"/>
@@ -32,8 +32,30 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={2FB3A80C-B0C8-4D8F-AB87-5FEA77D77874}</author>
+  </authors>
+  <commentList>
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{2FB3A80C-B0C8-4D8F-AB87-5FEA77D77874}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    test
+1=intro convo
+2="talk" selection
+3=exit convo?
+etc</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
   <si>
     <t>CONVERSATION_ID</t>
   </si>
@@ -69,16 +91,55 @@
   </si>
   <si>
     <t>Time (in seconds) (float)</t>
+  </si>
+  <si>
+    <t>ACTOR_NAME</t>
+  </si>
+  <si>
+    <t>joe</t>
+  </si>
+  <si>
+    <t>GOTO_CONVERSATION</t>
+  </si>
+  <si>
+    <t>GOTO_LINE</t>
+  </si>
+  <si>
+    <t>GOTO_SELECTION</t>
+  </si>
+  <si>
+    <t>SELECTION_ID</t>
+  </si>
+  <si>
+    <t>NUT</t>
+  </si>
+  <si>
+    <t>MEME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HELLO </t>
+  </si>
+  <si>
+    <t>j3fF</t>
+  </si>
+  <si>
+    <t>Exit</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -123,15 +184,27 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Aleks" id="{748CBDCF-800E-4341-8DDE-833EDC503FF5}" userId="Aleks" providerId="None"/>
+</personList>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{386ED1A0-201A-4F8B-B32E-4424A1FB643F}" name="Table1" displayName="Table1" ref="A1:F33" totalsRowShown="0">
-  <autoFilter ref="A1:F33" xr:uid="{B3735E38-D8D5-4836-AA59-2709AB67C6CD}"/>
-  <tableColumns count="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{386ED1A0-201A-4F8B-B32E-4424A1FB643F}" name="Table1" displayName="Table1" ref="A1:L11" totalsRowShown="0">
+  <autoFilter ref="A1:L11" xr:uid="{B3735E38-D8D5-4836-AA59-2709AB67C6CD}"/>
+  <tableColumns count="12">
     <tableColumn id="2" xr3:uid="{F6C94841-C46C-44B9-A572-A721F231645C}" name="ROW_ID"/>
+    <tableColumn id="7" xr3:uid="{58D4295E-E9C0-45D2-B6F0-F728210B5C20}" name="ACTOR_NAME"/>
     <tableColumn id="1" xr3:uid="{BD13C5C0-1F48-4EE5-98FB-D2F0FFE39190}" name="ACTOR_ID"/>
+    <tableColumn id="11" xr3:uid="{4CD280B1-22DE-4FD8-99A4-E553102BBD33}" name="SELECTION_ID"/>
     <tableColumn id="3" xr3:uid="{3B6C4319-AE86-47CF-BD7D-4266E82D5B24}" name="CONVERSATION_ID"/>
     <tableColumn id="4" xr3:uid="{74D0FA3D-98C6-4F58-8546-C43D4CF67BD9}" name="LINE_ID"/>
     <tableColumn id="5" xr3:uid="{8A3C3CC2-D561-4942-8319-D8EC8F88EF02}" name="Text"/>
+    <tableColumn id="8" xr3:uid="{3C1C3A60-4AD9-4CC1-8279-CAB05DBF84E5}" name="GOTO_CONVERSATION"/>
+    <tableColumn id="9" xr3:uid="{CA30DC81-1DA8-4987-AF9E-7D3B5C95CA9D}" name="GOTO_SELECTION"/>
+    <tableColumn id="10" xr3:uid="{729A9085-4053-483D-88BA-7721399EAB41}" name="GOTO_LINE"/>
+    <tableColumn id="12" xr3:uid="{85DA8213-960A-4384-80DC-A5469E2438E4}" name="Exit"/>
     <tableColumn id="6" xr3:uid="{3D137972-8068-4627-A0D4-D9934B36D5FA}" name="Time (in seconds) (float)"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -433,50 +506,86 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="D1" dT="2020-07-28T20:31:34.16" personId="{748CBDCF-800E-4341-8DDE-833EDC503FF5}" id="{2FB3A80C-B0C8-4D8F-AB87-5FEA77D77874}">
+    <text>test
+1=intro convo
+2="talk" selection
+3=exit convo?
+etc</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA6A0927-9E5D-4546-957E-A7E3585F4B76}">
-  <dimension ref="A1:F33"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA6A0927-9E5D-4546-957E-A7E3585F4B76}">
+  <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" customWidth="1"/>
-    <col min="3" max="3" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" customWidth="1"/>
-    <col min="6" max="6" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" customWidth="1"/>
+    <col min="8" max="8" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="25.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
       <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
       <c r="F1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>1</v>
+      <c r="B2" t="s">
+        <v>13</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -484,481 +593,292 @@
       <c r="D2">
         <v>1</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
         <v>4</v>
       </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="L2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3">
-        <v>1</v>
+      <c r="B3" t="s">
+        <v>13</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3">
-        <v>2</v>
-      </c>
-      <c r="E3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+      <c r="G3" t="s">
         <v>5</v>
       </c>
-      <c r="F3">
+      <c r="L3">
         <v>1.5</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4">
-        <v>1</v>
+      <c r="B4" t="s">
+        <v>13</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
         <v>3</v>
       </c>
-      <c r="E4" t="s">
+      <c r="G4" t="s">
         <v>6</v>
       </c>
-      <c r="F4">
+      <c r="L4">
         <v>1.5</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5">
-        <v>1</v>
+      <c r="B5" t="s">
+        <v>13</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
         <v>4</v>
       </c>
-      <c r="E5" t="s">
+      <c r="G5" t="s">
         <v>7</v>
       </c>
-      <c r="F5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="L5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6">
-        <v>1</v>
+      <c r="B6" t="s">
+        <v>13</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
         <v>5</v>
       </c>
-      <c r="E6" t="s">
+      <c r="G6" t="s">
         <v>8</v>
       </c>
-      <c r="F6">
+      <c r="L6">
         <v>1.5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7">
-        <v>1</v>
+      <c r="B7" t="s">
+        <v>13</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
       <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
         <v>6</v>
       </c>
-      <c r="E7" t="s">
+      <c r="G7" t="s">
         <v>9</v>
       </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H7">
+        <v>2</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+      <c r="L7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8">
-        <v>1</v>
+      <c r="B8" t="s">
+        <v>13</v>
       </c>
       <c r="C8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E8">
+        <v>2</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8" t="s">
+        <v>20</v>
+      </c>
+      <c r="L8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9">
-        <v>1</v>
+      <c r="B9" t="s">
+        <v>13</v>
       </c>
       <c r="C9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+      <c r="F9">
+        <v>2</v>
+      </c>
+      <c r="G9" t="s">
+        <v>18</v>
+      </c>
+      <c r="L9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10">
-        <v>1</v>
+      <c r="B10" t="s">
+        <v>13</v>
       </c>
       <c r="C10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>2</v>
+      </c>
+      <c r="F10">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G10" t="s">
+        <v>19</v>
+      </c>
+      <c r="H10">
+        <v>3</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10">
+        <v>1</v>
+      </c>
+      <c r="K10">
+        <v>1</v>
+      </c>
+      <c r="L10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11">
-        <v>1</v>
+      <c r="B11" t="s">
+        <v>13</v>
       </c>
       <c r="C11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D11">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12">
-        <v>1</v>
-      </c>
-      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="E11">
         <v>3</v>
       </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
-      <c r="C13">
-        <v>3</v>
-      </c>
-      <c r="D13">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14">
-        <v>1</v>
-      </c>
-      <c r="C14">
-        <v>3</v>
-      </c>
-      <c r="D14">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15">
-        <v>1</v>
-      </c>
-      <c r="C15">
-        <v>3</v>
-      </c>
-      <c r="D15">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16">
-        <v>1</v>
-      </c>
-      <c r="C16">
-        <v>3</v>
-      </c>
-      <c r="D16">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>16</v>
-      </c>
-      <c r="B17">
-        <v>1</v>
-      </c>
-      <c r="C17">
-        <v>3</v>
-      </c>
-      <c r="D17">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>17</v>
-      </c>
-      <c r="B18">
-        <v>1</v>
-      </c>
-      <c r="C18">
-        <v>3</v>
-      </c>
-      <c r="D18">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>18</v>
-      </c>
-      <c r="B19">
-        <v>1</v>
-      </c>
-      <c r="C19">
-        <v>4</v>
-      </c>
-      <c r="D19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>19</v>
-      </c>
-      <c r="B20">
-        <v>1</v>
-      </c>
-      <c r="C20">
-        <v>5</v>
-      </c>
-      <c r="D20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>20</v>
-      </c>
-      <c r="B21">
-        <v>1</v>
-      </c>
-      <c r="C21">
-        <v>6</v>
-      </c>
-      <c r="D21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22">
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11" t="s">
         <v>21</v>
       </c>
-      <c r="B22">
-        <v>1</v>
-      </c>
-      <c r="C22">
-        <v>7</v>
-      </c>
-      <c r="D22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>22</v>
-      </c>
-      <c r="B23">
-        <v>1</v>
-      </c>
-      <c r="C23">
-        <v>7</v>
-      </c>
-      <c r="D23">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>23</v>
-      </c>
-      <c r="B24">
-        <v>1</v>
-      </c>
-      <c r="C24">
-        <v>7</v>
-      </c>
-      <c r="D24">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>24</v>
-      </c>
-      <c r="B25">
-        <v>1</v>
-      </c>
-      <c r="C25">
-        <v>7</v>
-      </c>
-      <c r="D25">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>25</v>
-      </c>
-      <c r="B26">
-        <v>1</v>
-      </c>
-      <c r="C26">
-        <v>7</v>
-      </c>
-      <c r="D26">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>26</v>
-      </c>
-      <c r="B27">
-        <v>1</v>
-      </c>
-      <c r="C27">
-        <v>7</v>
-      </c>
-      <c r="D27">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>27</v>
-      </c>
-      <c r="B28">
-        <v>1</v>
-      </c>
-      <c r="C28">
-        <v>7</v>
-      </c>
-      <c r="D28">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>28</v>
-      </c>
-      <c r="B29">
-        <v>1</v>
-      </c>
-      <c r="C29">
-        <v>7</v>
-      </c>
-      <c r="D29">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>29</v>
-      </c>
-      <c r="B30">
-        <v>1</v>
-      </c>
-      <c r="C30">
-        <v>8</v>
-      </c>
-      <c r="D30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>30</v>
-      </c>
-      <c r="B31">
-        <v>1</v>
-      </c>
-      <c r="C31">
-        <v>8</v>
-      </c>
-      <c r="D31">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>31</v>
-      </c>
-      <c r="B32">
-        <v>1</v>
-      </c>
-      <c r="C32">
-        <v>9</v>
-      </c>
-      <c r="D32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>32</v>
-      </c>
-      <c r="B33">
-        <v>1</v>
-      </c>
-      <c r="C33">
-        <v>10</v>
-      </c>
-      <c r="D33">
-        <v>1</v>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+      <c r="J11">
+        <v>1</v>
+      </c>
+      <c r="L11">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>